<commit_message>
fix: added payment type
</commit_message>
<xml_diff>
--- a/files/customerCard.xlsx
+++ b/files/customerCard.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alsu\Desktop\eliana_price_server\files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Проекты\Элиана прайс-лист\eliana_price_server\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>@orderDate</t>
   </si>
@@ -60,6 +60,12 @@
   </si>
   <si>
     <t>@shortName</t>
+  </si>
+  <si>
+    <t>Тип оплаты</t>
+  </si>
+  <si>
+    <t>@paymentType</t>
   </si>
 </sst>
 </file>
@@ -236,15 +242,6 @@
     <xf numFmtId="49" fontId="1" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -267,23 +264,32 @@
     <xf numFmtId="49" fontId="1" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="2" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -571,156 +577,160 @@
       <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="11.21875" customWidth="1"/>
+    <col min="3" max="3" width="11.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="20" t="s">
+    <row r="1" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
-      <c r="E1" s="19"/>
-      <c r="F1" s="18"/>
-    </row>
-    <row r="2" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="17"/>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="14"/>
+    </row>
+    <row r="2" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="15"/>
       <c r="B2" s="16"/>
       <c r="C2" s="16"/>
       <c r="D2" s="16"/>
       <c r="E2" s="16"/>
-      <c r="F2" s="15"/>
-    </row>
-    <row r="3" spans="1:6" ht="18" x14ac:dyDescent="0.3">
-      <c r="A3" s="9"/>
-      <c r="B3" s="8"/>
-      <c r="C3" s="8"/>
-      <c r="D3" s="8"/>
-      <c r="E3" s="8"/>
-      <c r="F3" s="7"/>
-    </row>
-    <row r="4" spans="1:6" ht="18" x14ac:dyDescent="0.3">
-      <c r="A4" s="6" t="s">
+      <c r="F2" s="17"/>
+    </row>
+    <row r="3" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="6"/>
+      <c r="B3" s="5"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="4"/>
+    </row>
+    <row r="4" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="5"/>
-      <c r="C4" s="5" t="s">
+      <c r="B4" s="18"/>
+      <c r="C4" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5"/>
-      <c r="F4" s="4"/>
-    </row>
-    <row r="5" spans="1:6" ht="18" x14ac:dyDescent="0.3">
-      <c r="A5" s="9"/>
-      <c r="B5" s="8"/>
-      <c r="C5" s="8"/>
-      <c r="D5" s="8"/>
-      <c r="E5" s="8"/>
-      <c r="F5" s="7"/>
-    </row>
-    <row r="6" spans="1:6" ht="18" x14ac:dyDescent="0.3">
-      <c r="A6" s="6" t="s">
+      <c r="D4" s="18"/>
+      <c r="E4" s="18"/>
+      <c r="F4" s="19"/>
+    </row>
+    <row r="5" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="6"/>
+      <c r="B5" s="5"/>
+      <c r="C5" s="5"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="4"/>
+    </row>
+    <row r="6" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="5"/>
-      <c r="C6" s="5" t="s">
+      <c r="B6" s="18"/>
+      <c r="C6" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
-      <c r="F6" s="4"/>
-    </row>
-    <row r="7" spans="1:6" ht="18" x14ac:dyDescent="0.3">
-      <c r="A7" s="9"/>
-      <c r="B7" s="8"/>
-      <c r="C7" s="8"/>
-      <c r="D7" s="8"/>
-      <c r="E7" s="8"/>
-      <c r="F7" s="14"/>
-    </row>
-    <row r="8" spans="1:6" ht="18" x14ac:dyDescent="0.3">
-      <c r="A8" s="6" t="s">
+      <c r="D6" s="18"/>
+      <c r="E6" s="18"/>
+      <c r="F6" s="19"/>
+    </row>
+    <row r="7" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="6"/>
+      <c r="B7" s="5"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="11"/>
+    </row>
+    <row r="8" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="5"/>
-      <c r="C8" s="5" t="s">
+      <c r="B8" s="18"/>
+      <c r="C8" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5"/>
-      <c r="F8" s="4"/>
-    </row>
-    <row r="9" spans="1:6" ht="18" x14ac:dyDescent="0.3">
-      <c r="A9" s="9"/>
-      <c r="B9" s="8"/>
-      <c r="C9" s="8"/>
-      <c r="D9" s="8"/>
-      <c r="E9" s="8"/>
-      <c r="F9" s="14"/>
-    </row>
-    <row r="10" spans="1:6" ht="18" x14ac:dyDescent="0.3">
-      <c r="A10" s="9"/>
-      <c r="B10" s="8"/>
-      <c r="C10" s="8"/>
-      <c r="D10" s="8"/>
-      <c r="E10" s="8"/>
-      <c r="F10" s="14"/>
-    </row>
-    <row r="11" spans="1:6" ht="18" x14ac:dyDescent="0.3">
-      <c r="A11" s="6"/>
-      <c r="B11" s="5"/>
-      <c r="C11" s="5"/>
-      <c r="D11" s="5"/>
-      <c r="E11" s="5"/>
-      <c r="F11" s="4"/>
-    </row>
-    <row r="12" spans="1:6" ht="18" x14ac:dyDescent="0.3">
-      <c r="A12" s="13"/>
-      <c r="B12" s="12"/>
-      <c r="C12" s="12"/>
-      <c r="D12" s="12"/>
-      <c r="E12" s="12"/>
-      <c r="F12" s="11"/>
-    </row>
-    <row r="13" spans="1:6" ht="18" x14ac:dyDescent="0.3">
-      <c r="A13" s="6" t="s">
+      <c r="D8" s="18"/>
+      <c r="E8" s="18"/>
+      <c r="F8" s="19"/>
+    </row>
+    <row r="9" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A9" s="6"/>
+      <c r="B9" s="5"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="11"/>
+    </row>
+    <row r="10" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A10" s="6"/>
+      <c r="B10" s="5"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="5"/>
+      <c r="F10" s="11"/>
+    </row>
+    <row r="11" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A11" s="20"/>
+      <c r="B11" s="18"/>
+      <c r="C11" s="18"/>
+      <c r="D11" s="18"/>
+      <c r="E11" s="18"/>
+      <c r="F11" s="19"/>
+    </row>
+    <row r="12" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A12" s="10"/>
+      <c r="B12" s="9"/>
+      <c r="C12" s="9"/>
+      <c r="D12" s="9"/>
+      <c r="E12" s="9"/>
+      <c r="F12" s="8"/>
+    </row>
+    <row r="13" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A13" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="B13" s="5"/>
-      <c r="C13" s="10" t="s">
+      <c r="B13" s="18"/>
+      <c r="C13" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="D13" s="5" t="s">
+      <c r="D13" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="E13" s="5"/>
-      <c r="F13" s="4"/>
-    </row>
-    <row r="14" spans="1:6" ht="18" x14ac:dyDescent="0.3">
-      <c r="A14" s="9"/>
-      <c r="B14" s="8"/>
-      <c r="C14" s="8"/>
-      <c r="D14" s="8"/>
-      <c r="E14" s="8"/>
-      <c r="F14" s="7"/>
-    </row>
-    <row r="15" spans="1:6" ht="18" x14ac:dyDescent="0.3">
-      <c r="A15" s="6" t="s">
+      <c r="E13" s="18"/>
+      <c r="F13" s="19"/>
+    </row>
+    <row r="14" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A14" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14" s="18"/>
+      <c r="C14" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="D14" s="18"/>
+      <c r="E14" s="18"/>
+      <c r="F14" s="19"/>
+    </row>
+    <row r="15" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A15" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="B15" s="5"/>
-      <c r="C15" s="5" t="s">
+      <c r="B15" s="18"/>
+      <c r="C15" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="D15" s="5"/>
-      <c r="E15" s="5"/>
-      <c r="F15" s="4"/>
-    </row>
-    <row r="16" spans="1:6" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D15" s="18"/>
+      <c r="E15" s="18"/>
+      <c r="F15" s="19"/>
+    </row>
+    <row r="16" spans="1:6" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="3"/>
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
@@ -729,13 +739,7 @@
       <c r="F16" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="13">
-    <mergeCell ref="A1:F2"/>
-    <mergeCell ref="C4:F4"/>
-    <mergeCell ref="C6:F6"/>
-    <mergeCell ref="D13:F13"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A6:B6"/>
+  <mergeCells count="15">
     <mergeCell ref="A15:B15"/>
     <mergeCell ref="C15:F15"/>
     <mergeCell ref="A11:B11"/>
@@ -743,6 +747,14 @@
     <mergeCell ref="A8:B8"/>
     <mergeCell ref="C8:F8"/>
     <mergeCell ref="A13:B13"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="C14:F14"/>
+    <mergeCell ref="A1:F2"/>
+    <mergeCell ref="C4:F4"/>
+    <mergeCell ref="C6:F6"/>
+    <mergeCell ref="D13:F13"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A6:B6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>